<commit_message>
Addition of Crossings to PLC excel file and importing into Track Controller Updated to import crossings and display in crossing table on component tab and started to introduce switchin between red line and green line on summary tab
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/wayside_fun.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/wayside_fun.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38540" yWindow="2560" windowWidth="25400" windowHeight="15540" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="25400" windowHeight="15460" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="GREEN_SWITCHES" sheetId="9" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="RED_SWITCHES" sheetId="12" r:id="rId6"/>
     <sheet name="RED_12" sheetId="10" r:id="rId7"/>
     <sheet name="RED_6_11" sheetId="11" r:id="rId8"/>
-    <sheet name="Green Line Crossing" sheetId="8" r:id="rId9"/>
-    <sheet name="Red Line" sheetId="2" r:id="rId10"/>
-    <sheet name="Green Line" sheetId="4" r:id="rId11"/>
+    <sheet name="GREEN_CROSSING" sheetId="8" r:id="rId9"/>
+    <sheet name="RED_CROSSING" sheetId="13" r:id="rId10"/>
+    <sheet name="Red Line" sheetId="2" r:id="rId11"/>
+    <sheet name="Green Line" sheetId="4" r:id="rId12"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="183">
   <si>
     <t>D13:C12</t>
   </si>
@@ -556,6 +557,36 @@
   </si>
   <si>
     <t>E-16:STOP</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>SECTION</t>
+  </si>
+  <si>
+    <t>BLOCK</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>INACTIVE</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <t>RED</t>
   </si>
 </sst>
 </file>
@@ -638,7 +669,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -682,6 +713,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1214,6 +1248,62 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="17">
+        <v>47</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1244,19 +1334,19 @@
       <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" ht="26" x14ac:dyDescent="0.3">
       <c r="D2" s="3" t="s">
@@ -1598,7 +1688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S53"/>
   <sheetViews>
@@ -1618,18 +1708,18 @@
       <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
       <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
@@ -3172,10 +3262,10 @@
       <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="17"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="15" t="s">
         <v>146</v>
       </c>
@@ -4650,7 +4740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -4674,10 +4764,10 @@
       <c r="C1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="17"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="15" t="s">
         <v>146</v>
       </c>
@@ -5000,48 +5090,62 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="C1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>40</v>
-      </c>
+    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="17">
+        <v>19</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Addition of Track View
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/wayside_fun.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/wayside_fun.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylemonto/Documents/Pitt/Senior/COE 1186/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylemonto/Documents/Pitt/Senior/COE 1186/ECE1186/TrainSystem/src/com/rogueone/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="10"/>
+    <workbookView xWindow="7740" yWindow="4160" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="GREEN_SWITCHES" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="159">
   <si>
     <t>D13:C12</t>
   </si>
@@ -512,6 +512,9 @@
   </si>
   <si>
     <t>NEXT AND PREVIOUS BLOCK</t>
+  </si>
+  <si>
+    <t>Q-100:N-85</t>
   </si>
 </sst>
 </file>
@@ -1785,8 +1788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2009,8 +2012,8 @@
       <c r="E7" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="22" t="s">
-        <v>67</v>
+      <c r="F7" s="25" t="s">
+        <v>158</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>88</v>
@@ -2104,7 +2107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5306,7 +5309,7 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5442,7 +5445,7 @@
     </row>
     <row r="5" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="25" t="s">
         <v>146</v>
       </c>
       <c r="C5" s="8"/>

</xml_diff>

<commit_message>
Tweaked logic for evaluating proceeding, addition of activating crossings Modified Train Model to call an update of Track Controller when train is created Modified Wayside excel to include blocks that trigger activation of crossing
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/wayside_fun.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/wayside_fun.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="4160" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="7740" yWindow="4160" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="GREEN_SWITCHES" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="162">
   <si>
     <t>D13:C12</t>
   </si>
@@ -515,6 +515,15 @@
   </si>
   <si>
     <t>Q-100:N-85</t>
+  </si>
+  <si>
+    <t>ACTIVE BETWEEN</t>
+  </si>
+  <si>
+    <t>17,18,19,20,21</t>
+  </si>
+  <si>
+    <t>49,50,51,52,53,54,55,56,57,58,59</t>
   </si>
 </sst>
 </file>
@@ -628,7 +637,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -646,8 +655,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -726,13 +737,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="14" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
@@ -744,8 +755,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="16" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="20% - Accent1" xfId="11" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="12" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="13" builtinId="38"/>
@@ -757,11 +771,13 @@
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="68">
@@ -1788,7 +1804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2049,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2062,9 +2078,10 @@
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>154</v>
       </c>
@@ -2080,8 +2097,11 @@
       <c r="E1" s="18" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>135</v>
       </c>
@@ -2096,6 +2116,9 @@
       </c>
       <c r="E2" s="22" t="s">
         <v>134</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -6365,7 +6388,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6374,6 +6397,7 @@
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -6392,6 +6416,9 @@
       <c r="E1" s="18" t="s">
         <v>133</v>
       </c>
+      <c r="F1" s="34" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
@@ -6403,13 +6430,15 @@
       <c r="C2" s="31">
         <v>19</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="10"/>
+      <c r="F2" s="19" t="s">
+        <v>160</v>
+      </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -6422,13 +6451,14 @@
       <c r="P2" s="10"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified switch logic so trains can proceed even if train stopped on switch-block Modified track view to account for section J and the blocks in that section Included logic in wayside to manually operator a switch
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/wayside_fun.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/wayside_fun.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="4160" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="GREEN_SWITCHES" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="164">
   <si>
     <t>D13:C12</t>
   </si>
@@ -524,6 +524,12 @@
   </si>
   <si>
     <t>49,50,51,52,53,54,55,56,57,58,59</t>
+  </si>
+  <si>
+    <t>MANUAL SWITCHS - GREEN</t>
+  </si>
+  <si>
+    <t>3,</t>
   </si>
 </sst>
 </file>
@@ -637,7 +643,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -657,8 +663,10 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -749,17 +757,20 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="16" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="16" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="20% - Accent1" xfId="11" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="12" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="13" builtinId="38"/>
@@ -772,12 +783,14 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="68">
@@ -2067,7 +2080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2117,7 +2130,7 @@
       <c r="E2" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="36" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2130,15 +2143,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -2155,18 +2168,20 @@
       <c r="B1" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
+      <c r="C1" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
@@ -2175,7 +2190,9 @@
       <c r="B2" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="27" t="s">
+        <v>163</v>
+      </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -2577,6 +2594,7 @@
     <mergeCell ref="D1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2600,18 +2618,18 @@
       <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
       <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
@@ -4154,10 +4172,10 @@
       <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="35"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="18" t="s">
         <v>100</v>
       </c>
@@ -4447,10 +4465,10 @@
       <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="35"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="18" t="s">
         <v>100</v>
       </c>
@@ -4657,15 +4675,15 @@
       <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35" t="s">
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="35"/>
+      <c r="H1" s="37"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
@@ -5356,15 +5374,15 @@
       <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35" t="s">
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="35"/>
+      <c r="H1" s="37"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
@@ -5889,10 +5907,10 @@
       <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="35"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="18" t="s">
         <v>100</v>
       </c>
@@ -6046,15 +6064,15 @@
       <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35" t="s">
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="35"/>
+      <c r="H1" s="37"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -6388,7 +6406,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Start of Red Line Refactoring
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/wayside_fun.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/wayside_fun.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="2400" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="10"/>
+    <workbookView xWindow="8540" yWindow="2400" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GREEN_SWITCHES" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="207">
   <si>
     <t>D13:C12</t>
   </si>
@@ -352,18 +352,12 @@
     <t>E-15,J-52</t>
   </si>
   <si>
-    <t>U-77:C-9</t>
-  </si>
-  <si>
     <t>U-77:GO</t>
   </si>
   <si>
     <t>D-10:STOP</t>
   </si>
   <si>
-    <t>D-10:C-9</t>
-  </si>
-  <si>
     <t>U-77:STOP</t>
   </si>
   <si>
@@ -373,18 +367,12 @@
     <t>E-15</t>
   </si>
   <si>
-    <t>A-1:F-16</t>
-  </si>
-  <si>
     <t>C-9:STOP</t>
   </si>
   <si>
     <t>F-16:STOP</t>
   </si>
   <si>
-    <t>E-15:F-16</t>
-  </si>
-  <si>
     <t>F-16:GO</t>
   </si>
   <si>
@@ -397,9 +385,6 @@
     <t>J-53:STOP</t>
   </si>
   <si>
-    <t>N-66:J-52</t>
-  </si>
-  <si>
     <t>J-52:J-53</t>
   </si>
   <si>
@@ -418,9 +403,6 @@
     <t>J53_N66</t>
   </si>
   <si>
-    <t>E-16:STOP</t>
-  </si>
-  <si>
     <t>SECTION</t>
   </si>
   <si>
@@ -530,13 +512,160 @@
   </si>
   <si>
     <t>3,</t>
+  </si>
+  <si>
+    <t>MANUAL SWITCHS - RED</t>
+  </si>
+  <si>
+    <t>6,7,8,9,10,11,12</t>
+  </si>
+  <si>
+    <t>DEFAULT1</t>
+  </si>
+  <si>
+    <t>DEFAULT2</t>
+  </si>
+  <si>
+    <t>F-16:A-1</t>
+  </si>
+  <si>
+    <t>E-15:STOP</t>
+  </si>
+  <si>
+    <t>F-16:E-15</t>
+  </si>
+  <si>
+    <t>E-15:GO</t>
+  </si>
+  <si>
+    <t>H-27</t>
+  </si>
+  <si>
+    <t>H-27:H-28</t>
+  </si>
+  <si>
+    <t>H-27:GO</t>
+  </si>
+  <si>
+    <t>H-28:STOP</t>
+  </si>
+  <si>
+    <t>T-76:STOP</t>
+  </si>
+  <si>
+    <t>H-27:STOP</t>
+  </si>
+  <si>
+    <t>H-28:GO</t>
+  </si>
+  <si>
+    <t>H-27:T-76</t>
+  </si>
+  <si>
+    <t>T-76:GO</t>
+  </si>
+  <si>
+    <t>H-33</t>
+  </si>
+  <si>
+    <t>H-33:H-32</t>
+  </si>
+  <si>
+    <t>H-33:GO</t>
+  </si>
+  <si>
+    <t>H-32:STOP</t>
+  </si>
+  <si>
+    <t>R-72:STOP</t>
+  </si>
+  <si>
+    <t>H-33:STOP</t>
+  </si>
+  <si>
+    <t>H-32:GO</t>
+  </si>
+  <si>
+    <t>H-33:R-72</t>
+  </si>
+  <si>
+    <t>R-72:GO</t>
+  </si>
+  <si>
+    <t>H-38</t>
+  </si>
+  <si>
+    <t>H-38:H-39</t>
+  </si>
+  <si>
+    <t>H-38:GO</t>
+  </si>
+  <si>
+    <t>H-39:STOP</t>
+  </si>
+  <si>
+    <t>Q-71:STOP</t>
+  </si>
+  <si>
+    <t>H-38:STOP</t>
+  </si>
+  <si>
+    <t>H-39:GO</t>
+  </si>
+  <si>
+    <t>H-38:Q-71</t>
+  </si>
+  <si>
+    <t>Q-71:GO</t>
+  </si>
+  <si>
+    <t>H-44</t>
+  </si>
+  <si>
+    <t>H-44:H-43</t>
+  </si>
+  <si>
+    <t>H-44:GO</t>
+  </si>
+  <si>
+    <t>H-43:STOP</t>
+  </si>
+  <si>
+    <t>O-67:STOP</t>
+  </si>
+  <si>
+    <t>H-44:STOP</t>
+  </si>
+  <si>
+    <t>H-43:GO</t>
+  </si>
+  <si>
+    <t>H-44:O-67</t>
+  </si>
+  <si>
+    <t>O-67:GO</t>
+  </si>
+  <si>
+    <t>J-53:GO</t>
+  </si>
+  <si>
+    <t>J-52:N-66</t>
+  </si>
+  <si>
+    <t>C-9:U-77</t>
+  </si>
+  <si>
+    <t>C-9:GO</t>
+  </si>
+  <si>
+    <t>C-9:D-10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -589,8 +718,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -633,6 +777,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDEDED"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -666,7 +822,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -763,10 +919,20 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2042,7 +2208,7 @@
         <v>78</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>88</v>
@@ -2096,27 +2262,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>133</v>
-      </c>
       <c r="F1" s="34" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>42</v>
@@ -2125,13 +2291,13 @@
         <v>47</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2143,8 +2309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2152,6 +2318,7 @@
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -2163,37 +2330,41 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
+      <c r="D1" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="42" t="s">
+        <v>159</v>
+      </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
@@ -2590,9 +2761,6 @@
       <c r="N26" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:N1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -4172,10 +4340,10 @@
       <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="37"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="18" t="s">
         <v>100</v>
       </c>
@@ -4197,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>15</v>
@@ -4225,7 +4393,7 @@
     <row r="3" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="B3" s="22" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="21">
@@ -4465,10 +4633,10 @@
       <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="37"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="18" t="s">
         <v>100</v>
       </c>
@@ -4489,7 +4657,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>16</v>
@@ -4514,7 +4682,7 @@
     <row r="3" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="22" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="21">
@@ -4675,15 +4843,15 @@
       <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37" t="s">
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="38"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
@@ -4699,7 +4867,7 @@
         <v>96</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>97</v>
@@ -4729,7 +4897,7 @@
     <row r="3" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="16" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="24">
@@ -4757,7 +4925,7 @@
     <row r="4" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="15" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="24">
@@ -4785,7 +4953,7 @@
     <row r="5" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="16" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="24">
@@ -5374,15 +5542,15 @@
       <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37" t="s">
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="38"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
@@ -5398,7 +5566,7 @@
         <v>98</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>99</v>
@@ -5429,7 +5597,7 @@
     <row r="3" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="22" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="24">
@@ -5458,7 +5626,7 @@
     <row r="4" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="14" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="24">
@@ -5487,7 +5655,7 @@
     <row r="5" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="25" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="24">
@@ -5727,10 +5895,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5746,132 +5914,356 @@
     <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="L1" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="M1" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="N1" s="37" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>6</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>111</v>
+        <v>108</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>162</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>89</v>
       </c>
       <c r="E2" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="19">
+        <v>7</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="M3" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="19">
+        <v>8</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="L4" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="19">
+        <v>9</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="M5" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="19">
+        <v>10</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="M6" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="N6" s="26" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="19">
+        <v>11</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="F2" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="22" t="s">
+      <c r="E7" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" s="21" t="s">
+      <c r="F7" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="J2" s="21" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="19">
-        <v>11</v>
-      </c>
-      <c r="B3" s="20" t="s">
+      <c r="H7" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="J7" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3" s="21" t="s">
+      <c r="K7" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="L7" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="M7" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="N7" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="I3" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="19">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="19">
         <v>12</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B8" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C8" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="E8" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F8" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="H8" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="G4" s="22" t="s">
+      <c r="I8" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="M8" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="H4" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="I4" s="21" t="s">
+      <c r="N8" s="21" t="s">
         <v>109</v>
-      </c>
-      <c r="J4" s="21" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -5907,10 +6299,10 @@
       <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="37"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="18" t="s">
         <v>100</v>
       </c>
@@ -5920,7 +6312,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>101</v>
@@ -5938,7 +6330,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="25" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="26">
@@ -6064,15 +6456,15 @@
       <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37" t="s">
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="38"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -6084,7 +6476,7 @@
         <v>102</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>103</v>
@@ -6093,10 +6485,10 @@
         <v>19</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G2" s="19">
         <v>6</v>
@@ -6113,7 +6505,7 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="25" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="24">
@@ -6140,7 +6532,7 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="27" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="24">
@@ -6167,7 +6559,7 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="25" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="24">
@@ -6420,42 +6812,42 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>133</v>
-      </c>
       <c r="F1" s="34" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C2" s="31">
         <v>19</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>

</xml_diff>

<commit_message>
Updated to include track failures and stop train if block connected to switch is has failed. Changed lights on Red line Added menu bar items for green and red line track views
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/wayside_fun.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/wayside_fun.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="2560" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="6480" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GREEN_SWITCHES" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="205">
   <si>
     <t>D13:C12</t>
   </si>
@@ -362,12 +362,6 @@
   </si>
   <si>
     <t>E-15</t>
-  </si>
-  <si>
-    <t>C-9:STOP</t>
-  </si>
-  <si>
-    <t>F-16:STOP</t>
   </si>
   <si>
     <t>F-16:GO</t>
@@ -2208,7 +2202,7 @@
         <v>77</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>87</v>
@@ -2262,27 +2256,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>126</v>
-      </c>
       <c r="F1" s="34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>42</v>
@@ -2291,13 +2285,13 @@
         <v>47</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>127</v>
-      </c>
       <c r="F2" s="36" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2309,7 +2303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2330,16 +2324,16 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E1" s="38"/>
       <c r="F1" s="38"/>
@@ -2354,16 +2348,16 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -4365,7 +4359,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>15</v>
@@ -4393,7 +4387,7 @@
     <row r="3" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="B3" s="22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="21">
@@ -4657,7 +4651,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>16</v>
@@ -4682,7 +4676,7 @@
     <row r="3" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="21">
@@ -4867,7 +4861,7 @@
         <v>95</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>96</v>
@@ -4897,7 +4891,7 @@
     <row r="3" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="24">
@@ -4925,7 +4919,7 @@
     <row r="4" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="24">
@@ -4953,7 +4947,7 @@
     <row r="5" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="24">
@@ -5566,7 +5560,7 @@
         <v>97</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>98</v>
@@ -5597,7 +5591,7 @@
     <row r="3" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="24">
@@ -5626,7 +5620,7 @@
     <row r="4" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="24">
@@ -5655,7 +5649,7 @@
     <row r="5" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="25" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="24">
@@ -5897,8 +5891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5922,7 +5916,7 @@
         <v>31</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D1" s="37" t="s">
         <v>93</v>
@@ -5934,7 +5928,7 @@
         <v>93</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H1" s="37" t="s">
         <v>93</v>
@@ -5966,40 +5960,40 @@
         <v>107</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="21" t="s">
-        <v>109</v>
+      <c r="E2" s="26" t="s">
+        <v>108</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H2" s="26" t="s">
         <v>73</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J2" s="26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L2" s="21" t="s">
         <v>73</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N2" s="26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -6007,43 +6001,43 @@
         <v>7</v>
       </c>
       <c r="B3" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="E3" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="M3" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="I3" s="26" t="s">
+      <c r="N3" s="26" t="s">
         <v>170</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="L3" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="M3" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="N3" s="26" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -6051,43 +6045,43 @@
         <v>8</v>
       </c>
       <c r="B4" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="E4" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="L4" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="M4" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>175</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="I4" s="26" t="s">
+      <c r="N4" s="26" t="s">
         <v>179</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="K4" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="L4" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="N4" s="26" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -6095,43 +6089,43 @@
         <v>9</v>
       </c>
       <c r="B5" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="E5" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="M5" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="I5" s="26" t="s">
+      <c r="N5" s="26" t="s">
         <v>188</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="K5" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="L5" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="M5" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="N5" s="26" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -6139,43 +6133,43 @@
         <v>10</v>
       </c>
       <c r="B6" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="E6" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="M6" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>196</v>
-      </c>
-      <c r="I6" s="26" t="s">
+      <c r="N6" s="26" t="s">
         <v>197</v>
-      </c>
-      <c r="J6" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="K6" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="L6" s="26" t="s">
-        <v>196</v>
-      </c>
-      <c r="M6" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="N6" s="26" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -6183,43 +6177,43 @@
         <v>11</v>
       </c>
       <c r="B7" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="M7" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" s="21" t="s">
+      <c r="N7" s="21" t="s">
         <v>115</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="H7" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="I7" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="J7" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="K7" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="M7" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="N7" s="21" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -6230,7 +6224,7 @@
         <v>100</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>103</v>
@@ -6238,11 +6232,11 @@
       <c r="E8" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="21" t="s">
-        <v>108</v>
+      <c r="F8" s="26" t="s">
+        <v>201</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H8" s="26" t="s">
         <v>105</v>
@@ -6251,10 +6245,10 @@
         <v>104</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L8" s="21" t="s">
         <v>105</v>
@@ -6262,8 +6256,8 @@
       <c r="M8" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="21" t="s">
-        <v>108</v>
+      <c r="N8" s="26" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -6312,7 +6306,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>100</v>
@@ -6321,7 +6315,7 @@
         <v>53</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F2" s="19">
         <v>12</v>
@@ -6330,7 +6324,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="25" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="26">
@@ -6476,7 +6470,7 @@
         <v>101</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>102</v>
@@ -6485,10 +6479,10 @@
         <v>19</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G2" s="19">
         <v>6</v>
@@ -6505,7 +6499,7 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="24">
@@ -6532,7 +6526,7 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="24">
@@ -6559,7 +6553,7 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="24">
@@ -6812,42 +6806,42 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>126</v>
-      </c>
       <c r="F1" s="34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C2" s="31">
         <v>19</v>
       </c>
       <c r="D2" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="32" t="s">
-        <v>127</v>
-      </c>
       <c r="F2" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>

</xml_diff>